<commit_message>
performance logging + admin
</commit_message>
<xml_diff>
--- a/documentation/example_structure.xlsx
+++ b/documentation/example_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanapichpongsa/Documents/Finances/hsbc/NoAPI/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76014A1-5418-204A-9FA6-EE5E54D10FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EDB530-90FE-1A4F-8E6A-D9E428A175B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{1BC65E01-3840-1442-AB69-682D45ED626F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>2024 Annual Data</t>
   </si>
@@ -113,6 +113,9 @@
   <si>
     <t>PIZZA HUT</t>
   </si>
+  <si>
+    <t>total</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -255,40 +258,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -304,39 +278,11 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,12 +303,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -371,11 +327,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,6 +363,1660 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total_out</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$4:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>SubCategory_i</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SubCategory_i+1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3221-2E45-BD13-222E48072708}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>total_in</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$4:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>SubCategory_i</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SubCategory_i+1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$6:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D33-6F40-A7A5-214758F102D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5234CCA0-F85B-0F4F-312D-6BD355C316B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93CC42B3-9348-C3BA-8C5C-02BF730CB6C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,41 +2351,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
@@ -796,7 +2417,7 @@
       <c r="E6" s="10">
         <v>45</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -813,7 +2434,7 @@
       <c r="E7" s="10">
         <v>120</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="18" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
@@ -833,7 +2454,7 @@
       <c r="E8" s="10">
         <v>5.5</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -850,7 +2471,7 @@
       <c r="E9" s="10">
         <v>50</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -867,7 +2488,7 @@
       <c r="E10" s="10">
         <v>20</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -884,7 +2505,7 @@
       <c r="E11" s="10">
         <v>37.5</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -906,11 +2527,11 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
@@ -937,32 +2558,32 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="42">
+      <c r="E16" s="25">
         <f>F15-E14</f>
         <v>-128</v>
       </c>
-      <c r="F16" s="41"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="37"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
@@ -982,130 +2603,130 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="29">
+      <c r="B20" s="17">
         <v>1</v>
       </c>
       <c r="C20" s="6">
         <v>45667</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="22">
         <v>12.5</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="29">
+      <c r="B21" s="17">
         <v>2</v>
       </c>
       <c r="C21" s="7">
         <v>45669</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="22">
         <v>15</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="29">
+      <c r="B22" s="17">
         <v>3</v>
       </c>
       <c r="C22" s="7">
         <v>45671</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="22">
         <v>10.75</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="29">
+      <c r="B23" s="17">
         <v>4</v>
       </c>
       <c r="C23" s="7">
         <v>45673</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="22">
         <v>14.2</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="29">
+      <c r="B24" s="17">
         <v>5</v>
       </c>
       <c r="C24" s="7">
         <v>45677</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="22">
         <v>18.5</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="29">
+      <c r="B25" s="17">
         <v>6</v>
       </c>
       <c r="C25" s="7">
         <v>45682</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="22">
         <v>22</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="29">
+      <c r="B26" s="17">
         <v>7</v>
       </c>
       <c r="C26" s="7">
         <v>45685</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="22">
         <v>17.3</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
@@ -1113,11 +2734,11 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="34">
+      <c r="E28" s="22">
         <f>SUM(E20:E26)</f>
         <v>110.25</v>
       </c>
-      <c r="F28" s="28"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
@@ -1125,8 +2746,8 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="35">
+      <c r="E29" s="16"/>
+      <c r="F29" s="23">
         <f>SUM(F20:F26)</f>
         <v>0</v>
       </c>
@@ -1137,25 +2758,25 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="40">
+      <c r="E30" s="30">
         <f>F29-E28</f>
         <v>-110.25</v>
       </c>
       <c r="F30" s="31"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="20">
         <f>SUM(E14,E28)</f>
         <v>388.25</v>
       </c>
@@ -1173,21 +2794,21 @@
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="33">
+      <c r="B34" s="21">
         <f>SUM(E16,E30)</f>
         <v>-238.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B13:F13"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1195,148 +2816,163 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B33DB2-53DE-2D47-AD3A-047193AF7776}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="36"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="23"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="23"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="C4" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10">
+      <c r="B5" s="10">
         <f>Sheet1!E14</f>
         <v>278</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="C5" s="12">
+        <f>Sheet1!E28</f>
+        <v>110.25</v>
+      </c>
+      <c r="D5" s="39">
+        <f>Sheet1!B32</f>
+        <v>388.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="43">
+      <c r="B6" s="8">
         <f>Sheet1!F15</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
+      <c r="C6" s="9">
+        <f>Sheet1!F29</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <f>Sheet1!B33</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="44">
+      <c r="B7" s="21">
         <f>Sheet1!E16</f>
         <v>-128</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="12">
-        <f>Sheet1!E28</f>
-        <v>110.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="9">
-        <f>Sheet1!F29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="33">
+      <c r="C7" s="21">
         <f>Sheet1!E30</f>
         <v>-110.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="27">
-        <f>Sheet1!B32</f>
-        <v>388.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="26">
-        <f>Sheet1!B33</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="11">
+      <c r="D7" s="11">
         <f>Sheet1!B34</f>
         <v>-238.25</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="38"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="38"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="38"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A1:C2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>